<commit_message>
Fixed naming conventions of files
</commit_message>
<xml_diff>
--- a/MATLAB/FDTD/DataPath.xlsx
+++ b/MATLAB/FDTD/DataPath.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9036" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9036"/>
   </bookViews>
   <sheets>
     <sheet name="Raw FDTD Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="189">
   <si>
     <t>Simulation Folder</t>
   </si>
@@ -561,9 +561,6 @@
   </si>
   <si>
     <t>N:\Kat FDTD Data\Off Axis Quantification\SLAR MgF2 200 nm on glass for testing.xf\Simulations\000006\Run0001\output</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
   <si>
     <t>N:\Kat FDTD Data\Analyzed Data\Frequency Response\Free Space 700 to 1200 nm with 5 nm mesh.mat</t>
@@ -1078,23 +1075,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="120.6640625" customWidth="1"/>
-    <col min="2" max="2" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="93.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
     <col min="3" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="86.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="46.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="39.21875" bestFit="1" customWidth="1"/>
@@ -1139,10 +1137,10 @@
         <v>35</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1162,7 +1160,7 @@
         <v>1.92414E-17</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>700</v>
@@ -1171,22 +1169,22 @@
         <v>1200</v>
       </c>
       <c r="I2">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="J2">
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L2" t="s">
         <v>169</v>
       </c>
       <c r="M2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -1206,7 +1204,7 @@
         <v>9.6265399999999993E-18</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>700</v>
@@ -1215,22 +1213,22 @@
         <v>1200</v>
       </c>
       <c r="I3">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="J3">
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L3" t="s">
         <v>169</v>
       </c>
       <c r="M3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -1250,7 +1248,7 @@
         <v>9.6291700000000004E-18</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>700</v>
@@ -1259,22 +1257,22 @@
         <v>1200</v>
       </c>
       <c r="I4">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="J4">
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L4" t="s">
         <v>169</v>
       </c>
       <c r="M4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1294,7 +1292,7 @@
         <v>9.6291700000000004E-18</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>700</v>
@@ -1303,42 +1301,42 @@
         <v>1200</v>
       </c>
       <c r="I5">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="J5">
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L5" t="s">
         <v>169</v>
       </c>
       <c r="M5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C6">
         <v>1.5</v>
       </c>
       <c r="D6">
-        <v>3900</v>
+        <v>8400</v>
       </c>
       <c r="E6" s="3">
         <v>9.6291700000000004E-18</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>700</v>
@@ -1353,60 +1351,16 @@
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L6" t="s">
         <v>169</v>
       </c>
       <c r="M6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C7">
-        <v>1.5</v>
-      </c>
-      <c r="D7">
-        <v>8400</v>
-      </c>
-      <c r="E7" s="3">
-        <v>9.6291700000000004E-18</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>700</v>
-      </c>
-      <c r="H7">
-        <v>1200</v>
-      </c>
-      <c r="I7">
-        <v>120</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>181</v>
-      </c>
-      <c r="L7" t="s">
-        <v>169</v>
-      </c>
-      <c r="M7" t="s">
-        <v>189</v>
-      </c>
-      <c r="N7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1419,10 +1373,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1473,18 +1427,18 @@
         <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1514,10 +1468,10 @@
         <v>169</v>
       </c>
       <c r="L2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some unknown changes (HY)
</commit_message>
<xml_diff>
--- a/MATLAB/FDTD/DataPath.xlsx
+++ b/MATLAB/FDTD/DataPath.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="204">
   <si>
     <t>Simulation Folder</t>
   </si>
@@ -588,6 +588,51 @@
   </si>
   <si>
     <t>MultiPoint_Reflected_Light_Top_0_transient_</t>
+  </si>
+  <si>
+    <t>Free Space 300 to 1300 nm 5 nm mesh</t>
+  </si>
+  <si>
+    <t>MultiPoint_Reflected_Light_0_transient_</t>
+  </si>
+  <si>
+    <t>MultiPoint_Transmitted_Light_1_transient_</t>
+  </si>
+  <si>
+    <t>M:\Kat FDTD Data\2000 nm wide perm 225\free space 300 to 1300 nm.xf\Simulations\000002\Run0001\output</t>
+  </si>
+  <si>
+    <t>K:\FDTD\Slanted 7 layer IR mirror under waveguide with gap SILAR bottom top distant near field sensors.xf\Simulations\000002\Run0001\output</t>
+  </si>
+  <si>
+    <t>Slanted 7 layer mirror and waveguide new data analysis method</t>
+  </si>
+  <si>
+    <t>N:\Kat FDTD Data\Analyzed Data\Frequency Response\Free Space 300 to 1300 nm 5 nm mesh.mat</t>
+  </si>
+  <si>
+    <t>K:\FDTD\0-UCSC-NASA-Demaray\Slanted 7 layer IR mirror under waveguide with gap ARC top and bottom of layers distant sensors no -z padding.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>Slanted 7 layer mirror and waveguide no -z padding</t>
+  </si>
+  <si>
+    <t>K:\FDTD\0-UCSC-NASA-Demaray\Slanted 7 layer IR mirror in glass no waveguide. 10-7-14xf.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>Slanted 7 layer mirror in glass no waveguide 10 nm mesh</t>
+  </si>
+  <si>
+    <t>K:\FDTD\10-11-14  triangle grating in waveguide on glass slab from MATLAB suggestion #3 700-1200nm.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>Triangular grating, 250 nm height, 650 nm period, waveguide to air 25 nm mesh</t>
+  </si>
+  <si>
+    <t>Triangular grating, 250 nm height, 650 nm period, waveguide to air 10 nm mesh</t>
+  </si>
+  <si>
+    <t>K:\FDTD\10-12-14  triangle grating in waveguide on glass slab from MATLAB suggestion #3 700-1200nm slender.xf\Simulations\000002\Run0001\output</t>
   </si>
 </sst>
 </file>
@@ -661,10 +706,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -680,6 +724,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1075,71 +1125,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="93.33203125" customWidth="1"/>
+    <col min="1" max="1" width="154.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
     <col min="11" max="11" width="86.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="46.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="44.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="17" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1156,11 +1207,11 @@
       <c r="D2">
         <v>2400</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.92414E-17</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>700</v>
@@ -1200,11 +1251,11 @@
       <c r="D3">
         <v>4600</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>9.6265399999999993E-18</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>700</v>
@@ -1244,11 +1295,11 @@
       <c r="D4">
         <v>19400</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>9.6291700000000004E-18</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>700</v>
@@ -1288,11 +1339,11 @@
       <c r="D5">
         <v>3900</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>9.6291700000000004E-18</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>700</v>
@@ -1332,11 +1383,11 @@
       <c r="D6">
         <v>8400</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>9.6291700000000004E-18</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>700</v>
@@ -1360,6 +1411,227 @@
         <v>188</v>
       </c>
       <c r="N6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>77200</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.92547E-17</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>300</v>
+      </c>
+      <c r="H7">
+        <v>1300</v>
+      </c>
+      <c r="I7">
+        <v>200</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>195</v>
+      </c>
+      <c r="L7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M7" t="s">
+        <v>188</v>
+      </c>
+      <c r="N7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="D8">
+        <v>25000</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.92547E-17</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>300</v>
+      </c>
+      <c r="H8">
+        <v>1300</v>
+      </c>
+      <c r="I8">
+        <v>200</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>195</v>
+      </c>
+      <c r="L8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M8" t="s">
+        <v>188</v>
+      </c>
+      <c r="N8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
+      </c>
+      <c r="D9">
+        <v>25000</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.92566E-17</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>300</v>
+      </c>
+      <c r="H9">
+        <v>1300</v>
+      </c>
+      <c r="I9">
+        <v>200</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>195</v>
+      </c>
+      <c r="L9" t="s">
+        <v>169</v>
+      </c>
+      <c r="M9" t="s">
+        <v>188</v>
+      </c>
+      <c r="N9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10">
+        <v>1.5</v>
+      </c>
+      <c r="D10">
+        <v>10000</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.8145800000000002E-17</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>700</v>
+      </c>
+      <c r="H10">
+        <v>1200</v>
+      </c>
+      <c r="I10">
+        <f>10400/25</f>
+        <v>416</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>180</v>
+      </c>
+      <c r="L10" t="s">
+        <v>169</v>
+      </c>
+      <c r="M10" t="s">
+        <v>188</v>
+      </c>
+      <c r="N10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11">
+        <v>1.5</v>
+      </c>
+      <c r="D11">
+        <v>10000</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.9258299999999999E-17</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>700</v>
+      </c>
+      <c r="H11">
+        <v>1200</v>
+      </c>
+      <c r="I11">
+        <v>260</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>180</v>
+      </c>
+      <c r="L11" t="s">
+        <v>169</v>
+      </c>
+      <c r="M11" t="s">
+        <v>188</v>
+      </c>
+      <c r="N11" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1371,65 +1643,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.21875" customWidth="1"/>
     <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.77734375" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
     <col min="11" max="11" width="46.109375" customWidth="1"/>
     <col min="12" max="12" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="44.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="17" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1446,11 +1719,11 @@
       <c r="D2">
         <v>4000</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>9.6291700000000004E-18</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>700</v>
@@ -1472,6 +1745,47 @@
       </c>
       <c r="M2" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1100</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9.5958999999999999E-18</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>300</v>
+      </c>
+      <c r="H3">
+        <v>1300</v>
+      </c>
+      <c r="I3">
+        <v>200</v>
+      </c>
+      <c r="J3">
+        <v>200</v>
+      </c>
+      <c r="K3" t="s">
+        <v>169</v>
+      </c>
+      <c r="L3" t="s">
+        <v>190</v>
+      </c>
+      <c r="M3" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1484,35 +1798,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FN168"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="63.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="17.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:170" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:170" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0.124959853575387</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <f>B2*100</f>
         <v>12.4959853575387</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="5"/>
       <c r="F2">
         <v>0.124959853575387</v>
       </c>
@@ -2013,10 +2327,10 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.24878847535173601</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <f t="shared" ref="C3:C66" si="0">B3*100</f>
         <v>24.878847535173602</v>
       </c>
@@ -2025,10 +2339,10 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3.0895478503914199E-2</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <f t="shared" si="0"/>
         <v>3.08954785039142</v>
       </c>
@@ -2037,10 +2351,10 @@
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3.06837772913638E-2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <f t="shared" si="0"/>
         <v>3.0683777291363801</v>
       </c>
@@ -2049,10 +2363,10 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>1.4382143513319101E-2</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <f t="shared" si="0"/>
         <v>1.4382143513319101</v>
       </c>
@@ -2061,10 +2375,10 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>1.4073735748681499E-2</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <f t="shared" si="0"/>
         <v>1.40737357486815</v>
       </c>
@@ -2073,10 +2387,10 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>1.7598154056959199E-2</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <f t="shared" si="0"/>
         <v>1.7598154056959199</v>
       </c>
@@ -2085,10 +2399,10 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>1.7411819499078902E-2</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <f t="shared" si="0"/>
         <v>1.7411819499078902</v>
       </c>
@@ -2097,10 +2411,10 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>3.5111697957351203E-2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <f t="shared" si="0"/>
         <v>3.5111697957351202</v>
       </c>
@@ -2109,10 +2423,10 @@
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>3.4546924412749203E-2</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <f t="shared" si="0"/>
         <v>3.4546924412749203</v>
       </c>
@@ -2121,10 +2435,10 @@
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>3.1628202603985002E-2</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <f t="shared" si="0"/>
         <v>3.1628202603985001</v>
       </c>
@@ -2133,10 +2447,10 @@
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>3.1316729403351298E-2</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <f t="shared" si="0"/>
         <v>3.1316729403351298</v>
       </c>
@@ -2145,10 +2459,10 @@
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>6.5943644168223198E-3</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <f t="shared" si="0"/>
         <v>0.65943644168223203</v>
       </c>
@@ -2157,10 +2471,10 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>6.5085524933614896E-3</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <f t="shared" si="0"/>
         <v>0.65085524933614891</v>
       </c>
@@ -2169,10 +2483,10 @@
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>3.84830875820832E-2</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <f t="shared" si="0"/>
         <v>3.84830875820832</v>
       </c>
@@ -2181,10 +2495,10 @@
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>3.7762995559240703E-2</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <f t="shared" si="0"/>
         <v>3.7762995559240702</v>
       </c>
@@ -2193,10 +2507,10 @@
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>2.6644015478395601E-2</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <f t="shared" si="0"/>
         <v>2.6644015478395602</v>
       </c>
@@ -2205,10 +2519,10 @@
       <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>2.6246869502571699E-2</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <f t="shared" si="0"/>
         <v>2.6246869502571699</v>
       </c>
@@ -2217,10 +2531,10 @@
       <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>2.7584383683817899E-2</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <f t="shared" si="0"/>
         <v>2.7584383683817899</v>
       </c>
@@ -2229,10 +2543,10 @@
       <c r="A21" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>2.7584383683817899E-2</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <f t="shared" si="0"/>
         <v>2.7584383683817899</v>
       </c>
@@ -2241,10 +2555,10 @@
       <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>3.6126524276033203E-2</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <f t="shared" si="0"/>
         <v>3.6126524276033205</v>
       </c>
@@ -2253,10 +2567,10 @@
       <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>3.5660717958442202E-2</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <f t="shared" si="0"/>
         <v>3.5660717958442203</v>
       </c>
@@ -2265,10 +2579,10 @@
       <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>2.6531986539017501E-2</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <f t="shared" si="0"/>
         <v>2.6531986539017502</v>
       </c>
@@ -2277,10 +2591,10 @@
       <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>2.6257546260920899E-2</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <f t="shared" si="0"/>
         <v>2.6257546260920899</v>
       </c>
@@ -2289,10 +2603,10 @@
       <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>1.9984408749779799E-2</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8">
         <f t="shared" si="0"/>
         <v>1.9984408749779798</v>
       </c>
@@ -2301,10 +2615,10 @@
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>1.9852328106602299E-2</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <f t="shared" si="0"/>
         <v>1.9852328106602299</v>
       </c>
@@ -2313,10 +2627,10 @@
       <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>3.0895478503914199E-2</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <f t="shared" si="0"/>
         <v>3.08954785039142</v>
       </c>
@@ -2325,10 +2639,10 @@
       <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>3.06837772913638E-2</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <f t="shared" si="0"/>
         <v>3.0683777291363801</v>
       </c>
@@ -2337,10 +2651,10 @@
       <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>1.4382143513319101E-2</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <f t="shared" si="0"/>
         <v>1.4382143513319101</v>
       </c>
@@ -2349,10 +2663,10 @@
       <c r="A31" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>1.4073735748681499E-2</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8">
         <f t="shared" si="0"/>
         <v>1.40737357486815</v>
       </c>
@@ -2361,10 +2675,10 @@
       <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>1.7598154056959199E-2</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <f t="shared" si="0"/>
         <v>1.7598154056959199</v>
       </c>
@@ -2373,10 +2687,10 @@
       <c r="A33" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <v>1.7411819499078902E-2</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <f t="shared" si="0"/>
         <v>1.7411819499078902</v>
       </c>
@@ -2385,10 +2699,10 @@
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>4.6073174716479801E-2</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <f t="shared" si="0"/>
         <v>4.6073174716479803</v>
       </c>
@@ -2397,10 +2711,10 @@
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>4.6141306204415602E-2</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <f t="shared" si="0"/>
         <v>4.6141306204415606</v>
       </c>
@@ -2409,10 +2723,10 @@
       <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>2.2875577792782702E-2</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8">
         <f t="shared" si="0"/>
         <v>2.28755777927827</v>
       </c>
@@ -2421,10 +2735,10 @@
       <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <v>3.1636648746101503E-2</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <f t="shared" si="0"/>
         <v>3.1636648746101503</v>
       </c>
@@ -2433,10 +2747,10 @@
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <v>3.2959600350695298E-2</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8">
         <f t="shared" si="0"/>
         <v>3.2959600350695299</v>
       </c>
@@ -2445,10 +2759,10 @@
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="6">
         <v>3.4437567080522299E-2</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="8">
         <f t="shared" si="0"/>
         <v>3.4437567080522298</v>
       </c>
@@ -2457,10 +2771,10 @@
       <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="6">
         <v>1.8313208669586401E-2</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="8">
         <f t="shared" si="0"/>
         <v>1.83132086695864</v>
       </c>
@@ -2469,10 +2783,10 @@
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="6">
         <v>2.28106074270986E-2</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="8">
         <f t="shared" si="0"/>
         <v>2.2810607427098599</v>
       </c>
@@ -2481,10 +2795,10 @@
       <c r="A42" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="6">
         <v>2.3630441694765601E-2</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="8">
         <f t="shared" si="0"/>
         <v>2.3630441694765603</v>
       </c>
@@ -2493,10 +2807,10 @@
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="6">
         <v>6.4710620807345201E-2</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="8">
         <f t="shared" si="0"/>
         <v>6.4710620807345203</v>
       </c>
@@ -2505,10 +2819,10 @@
       <c r="A44" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <v>2.3684048657188699E-2</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="8">
         <f t="shared" si="0"/>
         <v>2.3684048657188699</v>
       </c>
@@ -2517,10 +2831,10 @@
       <c r="A45" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="6">
         <v>2.44385909598623E-2</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="8">
         <f t="shared" si="0"/>
         <v>2.4438590959862299</v>
       </c>
@@ -2529,10 +2843,10 @@
       <c r="A46" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="6">
         <v>4.1987493178762401E-2</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="8">
         <f t="shared" si="0"/>
         <v>4.1987493178762403</v>
       </c>
@@ -2541,10 +2855,10 @@
       <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="4">
         <v>4.5451633141674198E-2</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="8">
         <f t="shared" si="0"/>
         <v>4.5451633141674197</v>
       </c>
@@ -2553,10 +2867,10 @@
       <c r="A48" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="4">
         <v>4.0310985191116602E-2</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="8">
         <f t="shared" si="0"/>
         <v>4.0310985191116604</v>
       </c>
@@ -2565,10 +2879,10 @@
       <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="4">
         <v>4.2123302039144703E-2</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="8">
         <f t="shared" si="0"/>
         <v>4.2123302039144699</v>
       </c>
@@ -2577,10 +2891,10 @@
       <c r="A50" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="4">
         <v>4.09593967885373E-2</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="8">
         <f t="shared" si="0"/>
         <v>4.0959396788537301</v>
       </c>
@@ -2589,10 +2903,10 @@
       <c r="A51" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="4">
         <v>3.9872346058071197E-2</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="8">
         <f t="shared" si="0"/>
         <v>3.9872346058071195</v>
       </c>
@@ -2601,10 +2915,10 @@
       <c r="A52" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="4">
         <v>4.0786712221757802E-2</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="8">
         <f t="shared" si="0"/>
         <v>4.0786712221757799</v>
       </c>
@@ -2613,10 +2927,10 @@
       <c r="A53" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="4">
         <v>2.0819683601815801E-2</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="8">
         <f t="shared" si="0"/>
         <v>2.0819683601815799</v>
       </c>
@@ -2625,10 +2939,10 @@
       <c r="A54" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="7">
         <v>2.8466994686295599E-2</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="8">
         <f t="shared" si="0"/>
         <v>2.8466994686295601</v>
       </c>
@@ -2637,10 +2951,10 @@
       <c r="A55" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="7">
         <v>2.90160765257883E-2</v>
       </c>
-      <c r="C55" s="9">
+      <c r="C55" s="8">
         <f t="shared" si="0"/>
         <v>2.9016076525788299</v>
       </c>
@@ -2649,10 +2963,10 @@
       <c r="A56" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56" s="7">
         <v>3.06604800941946E-2</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="8">
         <f t="shared" si="0"/>
         <v>3.0660480094194602</v>
       </c>
@@ -2661,10 +2975,10 @@
       <c r="A57" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="8">
+      <c r="B57" s="7">
         <v>1.9938249987191899E-2</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C57" s="8">
         <f t="shared" si="0"/>
         <v>1.9938249987191898</v>
       </c>
@@ -2673,10 +2987,10 @@
       <c r="A58" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58" s="7">
         <v>2.0998896147571899E-2</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C58" s="8">
         <f t="shared" si="0"/>
         <v>2.0998896147571897</v>
       </c>
@@ -2685,10 +2999,10 @@
       <c r="A59" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59" s="7">
         <v>2.1436560551072101E-2</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="8">
         <f t="shared" si="0"/>
         <v>2.1436560551072104</v>
       </c>
@@ -2697,10 +3011,10 @@
       <c r="A60" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60" s="7">
         <v>3.9882935280051698E-2</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="8">
         <f t="shared" si="0"/>
         <v>3.9882935280051699</v>
       </c>
@@ -2709,10 +3023,10 @@
       <c r="A61" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B61" s="7">
         <v>2.3944052724692699E-2</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="8">
         <f t="shared" si="0"/>
         <v>2.3944052724692697</v>
       </c>
@@ -2721,10 +3035,10 @@
       <c r="A62" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62" s="7">
         <v>2.5201703299084902E-2</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="8">
         <f t="shared" si="0"/>
         <v>2.5201703299084901</v>
       </c>
@@ -2733,10 +3047,10 @@
       <c r="A63" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B63" s="4">
         <v>1.72627754682751E-2</v>
       </c>
-      <c r="C63" s="9">
+      <c r="C63" s="8">
         <f t="shared" si="0"/>
         <v>1.72627754682751</v>
       </c>
@@ -2745,10 +3059,10 @@
       <c r="A64" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="4">
         <v>2.96134263332042E-3</v>
       </c>
-      <c r="C64" s="9">
+      <c r="C64" s="8">
         <f t="shared" si="0"/>
         <v>0.29613426333204201</v>
       </c>
@@ -2757,10 +3071,10 @@
       <c r="A65" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="4">
         <v>6.47598739059527E-4</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="9">
         <f t="shared" si="0"/>
         <v>6.4759873905952697E-2</v>
       </c>
@@ -2769,10 +3083,10 @@
       <c r="A66" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="4">
         <v>3.2361459226220701E-4</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="9">
         <f t="shared" si="0"/>
         <v>3.2361459226220704E-2</v>
       </c>
@@ -2781,10 +3095,10 @@
       <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B67" s="4">
         <v>1.81426785933207E-2</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="8">
         <f t="shared" ref="C67:C130" si="1">B67*100</f>
         <v>1.81426785933207</v>
       </c>
@@ -2793,10 +3107,10 @@
       <c r="A68" t="s">
         <v>70</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="4">
         <v>3.4789318965079302E-3</v>
       </c>
-      <c r="C68" s="9">
+      <c r="C68" s="8">
         <f t="shared" si="1"/>
         <v>0.34789318965079302</v>
       </c>
@@ -2805,10 +3119,10 @@
       <c r="A69" t="s">
         <v>71</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B69" s="4">
         <v>1.34578749884603E-3</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C69" s="8">
         <f t="shared" si="1"/>
         <v>0.134578749884603</v>
       </c>
@@ -2817,10 +3131,10 @@
       <c r="A70" t="s">
         <v>72</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="4">
         <v>1.3848808110445599E-2</v>
       </c>
-      <c r="C70" s="9">
+      <c r="C70" s="8">
         <f t="shared" si="1"/>
         <v>1.3848808110445598</v>
       </c>
@@ -2829,10 +3143,10 @@
       <c r="A71" t="s">
         <v>66</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B71" s="4">
         <v>1.8177186390954701E-2</v>
       </c>
-      <c r="C71" s="9">
+      <c r="C71" s="8">
         <f t="shared" si="1"/>
         <v>1.81771863909547</v>
       </c>
@@ -2841,10 +3155,10 @@
       <c r="A72" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B72" s="4">
         <v>5.5167019692426598E-3</v>
       </c>
-      <c r="C72" s="9">
+      <c r="C72" s="8">
         <f t="shared" si="1"/>
         <v>0.551670196924266</v>
       </c>
@@ -2853,10 +3167,10 @@
       <c r="A73" t="s">
         <v>74</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B73" s="4">
         <v>2.6114202708692701E-2</v>
       </c>
-      <c r="C73" s="9">
+      <c r="C73" s="8">
         <f t="shared" si="1"/>
         <v>2.61142027086927</v>
       </c>
@@ -2865,10 +3179,10 @@
       <c r="A74" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="4">
         <v>1.9072293414228701E-2</v>
       </c>
-      <c r="C74" s="9">
+      <c r="C74" s="8">
         <f t="shared" si="1"/>
         <v>1.90722934142287</v>
       </c>
@@ -2877,10 +3191,10 @@
       <c r="A75" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="4">
         <v>1.71673234063313E-2</v>
       </c>
-      <c r="C75" s="9">
+      <c r="C75" s="8">
         <f t="shared" si="1"/>
         <v>1.7167323406331301</v>
       </c>
@@ -2889,10 +3203,10 @@
       <c r="A76" t="s">
         <v>77</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="4">
         <v>2.9564954222505001E-3</v>
       </c>
-      <c r="C76" s="9">
+      <c r="C76" s="8">
         <f t="shared" si="1"/>
         <v>0.29564954222505002</v>
       </c>
@@ -2901,10 +3215,10 @@
       <c r="A77" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="4">
         <v>6.4033631143796703E-4</v>
       </c>
-      <c r="C77" s="10">
+      <c r="C77" s="9">
         <f t="shared" si="1"/>
         <v>6.4033631143796704E-2</v>
       </c>
@@ -2913,10 +3227,10 @@
       <c r="A78" t="s">
         <v>79</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B78" s="4">
         <v>1.7304434199245399E-4</v>
       </c>
-      <c r="C78" s="10">
+      <c r="C78" s="9">
         <f t="shared" si="1"/>
         <v>1.7304434199245398E-2</v>
       </c>
@@ -2925,10 +3239,10 @@
       <c r="A79" t="s">
         <v>80</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="4">
         <v>1.8202043132267798E-2</v>
       </c>
-      <c r="C79" s="9">
+      <c r="C79" s="8">
         <f t="shared" si="1"/>
         <v>1.8202043132267798</v>
       </c>
@@ -2937,10 +3251,10 @@
       <c r="A80" t="s">
         <v>81</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="4">
         <v>3.50126318346287E-3</v>
       </c>
-      <c r="C80" s="9">
+      <c r="C80" s="8">
         <f t="shared" si="1"/>
         <v>0.35012631834628699</v>
       </c>
@@ -2949,10 +3263,10 @@
       <c r="A81" t="s">
         <v>82</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B81" s="4">
         <v>7.0757180265048996E-4</v>
       </c>
-      <c r="C81" s="10">
+      <c r="C81" s="9">
         <f t="shared" si="1"/>
         <v>7.0757180265048999E-2</v>
       </c>
@@ -2961,10 +3275,10 @@
       <c r="A82" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="4">
         <v>3.7943205817123098E-4</v>
       </c>
-      <c r="C82" s="10">
+      <c r="C82" s="9">
         <f t="shared" si="1"/>
         <v>3.7943205817123099E-2</v>
       </c>
@@ -2973,10 +3287,10 @@
       <c r="A83" t="s">
         <v>84</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B83" s="4">
         <v>1.8308605923006101E-2</v>
       </c>
-      <c r="C83" s="9">
+      <c r="C83" s="8">
         <f t="shared" si="1"/>
         <v>1.83086059230061</v>
       </c>
@@ -2985,10 +3299,10 @@
       <c r="A84" t="s">
         <v>85</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="4">
         <v>3.55764734455165E-3</v>
       </c>
-      <c r="C84" s="9">
+      <c r="C84" s="8">
         <f t="shared" si="1"/>
         <v>0.35576473445516499</v>
       </c>
@@ -2997,10 +3311,10 @@
       <c r="A85" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="4">
         <v>1.4093595082260301E-3</v>
       </c>
-      <c r="C85" s="9">
+      <c r="C85" s="8">
         <f t="shared" si="1"/>
         <v>0.14093595082260302</v>
       </c>
@@ -3009,10 +3323,10 @@
       <c r="A86" t="s">
         <v>87</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B86" s="4">
         <v>1.4056935904359901E-2</v>
       </c>
-      <c r="C86" s="9">
+      <c r="C86" s="8">
         <f t="shared" si="1"/>
         <v>1.4056935904359902</v>
       </c>
@@ -3021,10 +3335,10 @@
       <c r="A87" t="s">
         <v>88</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B87" s="4">
         <v>1.5876357664347501E-2</v>
       </c>
-      <c r="C87" s="9">
+      <c r="C87" s="8">
         <f t="shared" si="1"/>
         <v>1.58763576643475</v>
       </c>
@@ -3033,10 +3347,10 @@
       <c r="A88" t="s">
         <v>89</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B88" s="4">
         <v>3.33781788081406E-3</v>
       </c>
-      <c r="C88" s="9">
+      <c r="C88" s="8">
         <f t="shared" si="1"/>
         <v>0.33378178808140602</v>
       </c>
@@ -3045,10 +3359,10 @@
       <c r="A89" t="s">
         <v>90</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B89" s="4">
         <v>1.63145611520727E-3</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C89" s="8">
         <f t="shared" si="1"/>
         <v>0.16314561152072701</v>
       </c>
@@ -3057,10 +3371,10 @@
       <c r="A90" t="s">
         <v>91</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B90" s="4">
         <v>1.2618378453879901E-3</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C90" s="8">
         <f t="shared" si="1"/>
         <v>0.126183784538799</v>
       </c>
@@ -3069,10 +3383,10 @@
       <c r="A91" t="s">
         <v>92</v>
       </c>
-      <c r="B91" s="5">
+      <c r="B91" s="4">
         <v>1.6724542752597299E-2</v>
       </c>
-      <c r="C91" s="9">
+      <c r="C91" s="8">
         <f t="shared" si="1"/>
         <v>1.6724542752597298</v>
       </c>
@@ -3081,10 +3395,10 @@
       <c r="A92" t="s">
         <v>93</v>
       </c>
-      <c r="B92" s="5">
+      <c r="B92" s="4">
         <v>4.19437552985461E-3</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C92" s="8">
         <f t="shared" si="1"/>
         <v>0.41943755298546098</v>
       </c>
@@ -3093,10 +3407,10 @@
       <c r="A93" t="s">
         <v>94</v>
       </c>
-      <c r="B93" s="5">
+      <c r="B93" s="4">
         <v>1.89023497111208E-3</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C93" s="8">
         <f t="shared" si="1"/>
         <v>0.189023497111208</v>
       </c>
@@ -3105,10 +3419,10 @@
       <c r="A94" t="s">
         <v>95</v>
       </c>
-      <c r="B94" s="5">
+      <c r="B94" s="4">
         <v>1.48051710973693E-3</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="8">
         <f t="shared" si="1"/>
         <v>0.14805171097369299</v>
       </c>
@@ -3117,10 +3431,10 @@
       <c r="A95" t="s">
         <v>96</v>
       </c>
-      <c r="B95" s="5">
+      <c r="B95" s="4">
         <v>1.6597892883940601E-2</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C95" s="8">
         <f t="shared" si="1"/>
         <v>1.6597892883940601</v>
       </c>
@@ -3129,10 +3443,10 @@
       <c r="A96" t="s">
         <v>97</v>
       </c>
-      <c r="B96" s="5">
+      <c r="B96" s="4">
         <v>3.75765520794267E-3</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C96" s="8">
         <f t="shared" si="1"/>
         <v>0.37576552079426701</v>
       </c>
@@ -3141,10 +3455,10 @@
       <c r="A97" t="s">
         <v>98</v>
       </c>
-      <c r="B97" s="5">
+      <c r="B97" s="4">
         <v>1.63900170788155E-3</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C97" s="8">
         <f t="shared" si="1"/>
         <v>0.163900170788155</v>
       </c>
@@ -3153,10 +3467,10 @@
       <c r="A98" t="s">
         <v>99</v>
       </c>
-      <c r="B98" s="5">
+      <c r="B98" s="4">
         <v>2.32703780948275E-3</v>
       </c>
-      <c r="C98" s="9">
+      <c r="C98" s="8">
         <f t="shared" si="1"/>
         <v>0.23270378094827501</v>
       </c>
@@ -3165,10 +3479,10 @@
       <c r="A99" t="s">
         <v>101</v>
       </c>
-      <c r="B99" s="5">
+      <c r="B99" s="4">
         <v>1.5730350474484601E-2</v>
       </c>
-      <c r="C99" s="9">
+      <c r="C99" s="8">
         <f t="shared" si="1"/>
         <v>1.5730350474484602</v>
       </c>
@@ -3177,10 +3491,10 @@
       <c r="A100" t="s">
         <v>102</v>
       </c>
-      <c r="B100" s="5">
+      <c r="B100" s="4">
         <v>3.0377706834387899E-3</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C100" s="8">
         <f t="shared" si="1"/>
         <v>0.30377706834387896</v>
       </c>
@@ -3189,10 +3503,10 @@
       <c r="A101" t="s">
         <v>103</v>
       </c>
-      <c r="B101" s="5">
+      <c r="B101" s="4">
         <v>1.43750439190442E-3</v>
       </c>
-      <c r="C101" s="9">
+      <c r="C101" s="8">
         <f t="shared" si="1"/>
         <v>0.143750439190442</v>
       </c>
@@ -3201,10 +3515,10 @@
       <c r="A102" t="s">
         <v>104</v>
       </c>
-      <c r="B102" s="5">
+      <c r="B102" s="4">
         <v>1.0833157048046301E-3</v>
       </c>
-      <c r="C102" s="9">
+      <c r="C102" s="8">
         <f t="shared" si="1"/>
         <v>0.108331570480463</v>
       </c>
@@ -3213,10 +3527,10 @@
       <c r="A103" t="s">
         <v>100</v>
       </c>
-      <c r="B103" s="5">
+      <c r="B103" s="4">
         <v>1.5129412664507199E-2</v>
       </c>
-      <c r="C103" s="9">
+      <c r="C103" s="8">
         <f t="shared" si="1"/>
         <v>1.51294126645072</v>
       </c>
@@ -3225,10 +3539,10 @@
       <c r="A104" t="s">
         <v>105</v>
       </c>
-      <c r="B104" s="5">
+      <c r="B104" s="4">
         <v>3.44429473164819E-3</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C104" s="8">
         <f t="shared" si="1"/>
         <v>0.34442947316481898</v>
       </c>
@@ -3237,10 +3551,10 @@
       <c r="A105" t="s">
         <v>106</v>
       </c>
-      <c r="B105" s="5">
+      <c r="B105" s="4">
         <v>1.5574502596714E-3</v>
       </c>
-      <c r="C105" s="9">
+      <c r="C105" s="8">
         <f t="shared" si="1"/>
         <v>0.15574502596713999</v>
       </c>
@@ -3249,23 +3563,23 @@
       <c r="A106" t="s">
         <v>107</v>
       </c>
-      <c r="B106" s="5">
+      <c r="B106" s="4">
         <v>2.2815679573804102E-3</v>
       </c>
-      <c r="C106" s="9">
+      <c r="C106" s="8">
         <f t="shared" si="1"/>
         <v>0.22815679573804101</v>
       </c>
-      <c r="D106" s="6"/>
+      <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>108</v>
       </c>
-      <c r="B107" s="5">
+      <c r="B107" s="4">
         <v>1.6436516054704899E-2</v>
       </c>
-      <c r="C107" s="9">
+      <c r="C107" s="8">
         <f t="shared" si="1"/>
         <v>1.6436516054704899</v>
       </c>
@@ -3274,10 +3588,10 @@
       <c r="A108" t="s">
         <v>109</v>
       </c>
-      <c r="B108" s="5">
+      <c r="B108" s="4">
         <v>3.8128305414974299E-3</v>
       </c>
-      <c r="C108" s="9">
+      <c r="C108" s="8">
         <f t="shared" si="1"/>
         <v>0.38128305414974301</v>
       </c>
@@ -3286,10 +3600,10 @@
       <c r="A109" t="s">
         <v>110</v>
       </c>
-      <c r="B109" s="5">
+      <c r="B109" s="4">
         <v>5.3513425127889704E-3</v>
       </c>
-      <c r="C109" s="9">
+      <c r="C109" s="8">
         <f t="shared" si="1"/>
         <v>0.53513425127889702</v>
       </c>
@@ -3298,370 +3612,370 @@
       <c r="A110" t="s">
         <v>111</v>
       </c>
-      <c r="B110" s="5">
+      <c r="B110" s="4">
         <v>6.4069506438621596E-3</v>
       </c>
-      <c r="C110" s="9">
+      <c r="C110" s="8">
         <f t="shared" si="1"/>
         <v>0.64069506438621593</v>
       </c>
     </row>
-    <row r="111" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="12" t="s">
+    <row r="111" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B111" s="13">
+      <c r="B111" s="12">
         <v>8.6824363588499202E-3</v>
       </c>
-      <c r="C111" s="14">
+      <c r="C111" s="13">
         <f t="shared" si="1"/>
         <v>0.86824363588499198</v>
       </c>
     </row>
-    <row r="112" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="12" t="s">
+    <row r="112" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B112" s="13">
+      <c r="B112" s="12">
         <v>2.54483610833624E-2</v>
       </c>
-      <c r="C112" s="14">
+      <c r="C112" s="13">
         <f t="shared" si="1"/>
         <v>2.5448361083362401</v>
       </c>
     </row>
-    <row r="113" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="12" t="s">
+    <row r="113" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B113" s="13">
+      <c r="B113" s="12">
         <v>3.6059263937907697E-2</v>
       </c>
-      <c r="C113" s="14">
+      <c r="C113" s="13">
         <f t="shared" si="1"/>
         <v>3.6059263937907695</v>
       </c>
     </row>
-    <row r="114" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="12" t="s">
+    <row r="114" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B114" s="13">
+      <c r="B114" s="12">
         <v>4.1106665293225597E-2</v>
       </c>
-      <c r="C114" s="14">
+      <c r="C114" s="13">
         <f t="shared" si="1"/>
         <v>4.1106665293225593</v>
       </c>
     </row>
-    <row r="115" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="12" t="s">
+    <row r="115" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B115" s="13">
+      <c r="B115" s="12">
         <v>3.0303154326522402E-2</v>
       </c>
-      <c r="C115" s="14">
+      <c r="C115" s="13">
         <f t="shared" si="1"/>
         <v>3.0303154326522401</v>
       </c>
     </row>
-    <row r="116" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="12" t="s">
+    <row r="116" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B116" s="13">
+      <c r="B116" s="12">
         <v>3.7181925958224699E-2</v>
       </c>
-      <c r="C116" s="14">
+      <c r="C116" s="13">
         <f t="shared" si="1"/>
         <v>3.7181925958224697</v>
       </c>
     </row>
-    <row r="117" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="12" t="s">
+    <row r="117" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B117" s="13">
+      <c r="B117" s="12">
         <v>2.74505781958648E-2</v>
       </c>
-      <c r="C117" s="14">
+      <c r="C117" s="13">
         <f t="shared" si="1"/>
         <v>2.7450578195864801</v>
       </c>
     </row>
-    <row r="118" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="12" t="s">
+    <row r="118" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B118" s="13">
+      <c r="B118" s="12">
         <v>2.7284012141194601E-2</v>
       </c>
-      <c r="C118" s="14">
+      <c r="C118" s="13">
         <f t="shared" si="1"/>
         <v>2.7284012141194602</v>
       </c>
     </row>
-    <row r="119" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="12" t="s">
+    <row r="119" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B119" s="13">
+      <c r="B119" s="12">
         <v>2.6134119779441401E-2</v>
       </c>
-      <c r="C119" s="14">
+      <c r="C119" s="13">
         <f t="shared" si="1"/>
         <v>2.61341197794414</v>
       </c>
     </row>
-    <row r="120" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="12" t="s">
+    <row r="120" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B120" s="13">
+      <c r="B120" s="12">
         <v>5.0970613522234899E-2</v>
       </c>
-      <c r="C120" s="14">
+      <c r="C120" s="13">
         <f t="shared" si="1"/>
         <v>5.0970613522234895</v>
       </c>
     </row>
-    <row r="121" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="12" t="s">
+    <row r="121" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B121" s="13">
+      <c r="B121" s="12">
         <v>1.6499633527130301E-2</v>
       </c>
-      <c r="C121" s="14">
+      <c r="C121" s="13">
         <f t="shared" si="1"/>
         <v>1.6499633527130302</v>
       </c>
     </row>
-    <row r="122" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="12" t="s">
+    <row r="122" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B122" s="13">
+      <c r="B122" s="12">
         <v>2.4189976352871199E-2</v>
       </c>
-      <c r="C122" s="14">
+      <c r="C122" s="13">
         <f t="shared" si="1"/>
         <v>2.4189976352871199</v>
       </c>
     </row>
-    <row r="123" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="12" t="s">
+    <row r="123" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B123" s="13">
+      <c r="B123" s="12">
         <v>1.6045473277687499E-2</v>
       </c>
-      <c r="C123" s="14">
+      <c r="C123" s="13">
         <f t="shared" si="1"/>
         <v>1.6045473277687499</v>
       </c>
     </row>
-    <row r="124" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="12" t="s">
+    <row r="124" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B124" s="13">
+      <c r="B124" s="12">
         <v>1.17897191648104E-2</v>
       </c>
-      <c r="C124" s="14">
+      <c r="C124" s="13">
         <f t="shared" si="1"/>
         <v>1.1789719164810399</v>
       </c>
     </row>
-    <row r="125" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="12" t="s">
+    <row r="125" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B125" s="13">
+      <c r="B125" s="12">
         <v>1.3875262815485101E-2</v>
       </c>
-      <c r="C125" s="14">
+      <c r="C125" s="13">
         <f t="shared" si="1"/>
         <v>1.3875262815485101</v>
       </c>
     </row>
-    <row r="126" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="12" t="s">
+    <row r="126" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B126" s="13">
+      <c r="B126" s="12">
         <v>4.5732234170938198E-2</v>
       </c>
-      <c r="C126" s="14">
+      <c r="C126" s="13">
         <f t="shared" si="1"/>
         <v>4.5732234170938195</v>
       </c>
     </row>
-    <row r="127" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="12" t="s">
+    <row r="127" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B127" s="13">
+      <c r="B127" s="12">
         <v>1.33059091860704E-2</v>
       </c>
-      <c r="C127" s="14">
+      <c r="C127" s="13">
         <f t="shared" si="1"/>
         <v>1.3305909186070399</v>
       </c>
     </row>
-    <row r="128" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="12" t="s">
+    <row r="128" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B128" s="13">
+      <c r="B128" s="12">
         <v>2.14717558280813E-2</v>
       </c>
-      <c r="C128" s="14">
+      <c r="C128" s="13">
         <f t="shared" si="1"/>
         <v>2.14717558280813</v>
       </c>
     </row>
-    <row r="129" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="15" t="s">
+    <row r="129" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="B129" s="16">
+      <c r="B129" s="15">
         <v>3.0789627897639001E-2</v>
       </c>
-      <c r="C129" s="17">
+      <c r="C129" s="16">
         <f t="shared" si="1"/>
         <v>3.0789627897639003</v>
       </c>
     </row>
-    <row r="130" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="15" t="s">
+    <row r="130" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B130" s="16">
+      <c r="B130" s="15">
         <v>1.4227939631000301E-2</v>
       </c>
-      <c r="C130" s="17">
+      <c r="C130" s="16">
         <f t="shared" si="1"/>
         <v>1.4227939631000301</v>
       </c>
     </row>
-    <row r="131" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="15" t="s">
+    <row r="131" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B131" s="16">
+      <c r="B131" s="15">
         <v>1.7504986778019101E-2</v>
       </c>
-      <c r="C131" s="17">
+      <c r="C131" s="16">
         <f t="shared" ref="C131:C168" si="2">B131*100</f>
         <v>1.75049867780191</v>
       </c>
     </row>
-    <row r="132" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="15" t="s">
+    <row r="132" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B132" s="16">
+      <c r="B132" s="15">
         <v>3.4829311185050102E-2</v>
       </c>
-      <c r="C132" s="17">
+      <c r="C132" s="16">
         <f t="shared" si="2"/>
         <v>3.48293111850501</v>
       </c>
     </row>
-    <row r="133" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="15" t="s">
+    <row r="133" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B133" s="16">
+      <c r="B133" s="15">
         <v>3.1472466003668098E-2</v>
       </c>
-      <c r="C133" s="17">
+      <c r="C133" s="16">
         <f t="shared" si="2"/>
         <v>3.1472466003668096</v>
       </c>
     </row>
-    <row r="134" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="15" t="s">
+    <row r="134" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="B134" s="16">
+      <c r="B134" s="15">
         <v>6.5514584550919004E-3</v>
       </c>
-      <c r="C134" s="17">
+      <c r="C134" s="16">
         <f t="shared" si="2"/>
         <v>0.65514584550919008</v>
       </c>
     </row>
-    <row r="135" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="15" t="s">
+    <row r="135" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B135" s="16">
+      <c r="B135" s="15">
         <v>3.8123041570662E-2</v>
       </c>
-      <c r="C135" s="17">
+      <c r="C135" s="16">
         <f t="shared" si="2"/>
         <v>3.8123041570662002</v>
       </c>
     </row>
-    <row r="136" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="15" t="s">
+    <row r="136" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="B136" s="16">
+      <c r="B136" s="15">
         <v>2.6445442490483601E-2</v>
       </c>
-      <c r="C136" s="17">
+      <c r="C136" s="16">
         <f t="shared" si="2"/>
         <v>2.6445442490483599</v>
       </c>
     </row>
-    <row r="137" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="15" t="s">
+    <row r="137" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B137" s="16">
+      <c r="B137" s="15">
         <v>2.7584383683817899E-2</v>
       </c>
-      <c r="C137" s="17">
+      <c r="C137" s="16">
         <f t="shared" si="2"/>
         <v>2.7584383683817899</v>
       </c>
     </row>
-    <row r="138" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="15" t="s">
+    <row r="138" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="B138" s="16">
+      <c r="B138" s="15">
         <v>3.5893621117237803E-2</v>
       </c>
-      <c r="C138" s="17">
+      <c r="C138" s="16">
         <f t="shared" si="2"/>
         <v>3.5893621117237804</v>
       </c>
     </row>
-    <row r="139" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="15" t="s">
+    <row r="139" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="B139" s="16">
+      <c r="B139" s="15">
         <v>2.63947663999692E-2</v>
       </c>
-      <c r="C139" s="17">
+      <c r="C139" s="16">
         <f t="shared" si="2"/>
         <v>2.6394766399969201</v>
       </c>
     </row>
-    <row r="140" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="15" t="s">
+    <row r="140" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="B140" s="16">
+      <c r="B140" s="15">
         <v>1.9918368428191099E-2</v>
       </c>
-      <c r="C140" s="17">
+      <c r="C140" s="16">
         <f t="shared" si="2"/>
         <v>1.99183684281911</v>
       </c>
@@ -3670,10 +3984,10 @@
       <c r="A141" t="s">
         <v>166</v>
       </c>
-      <c r="B141" s="5">
+      <c r="B141" s="4">
         <v>1.2510517392676199E-2</v>
       </c>
-      <c r="C141" s="9">
+      <c r="C141" s="8">
         <f t="shared" si="2"/>
         <v>1.2510517392676199</v>
       </c>
@@ -3682,10 +3996,10 @@
       <c r="A142" t="s">
         <v>167</v>
       </c>
-      <c r="B142" s="5">
+      <c r="B142" s="4">
         <v>9.5277450358187601E-3</v>
       </c>
-      <c r="C142" s="9">
+      <c r="C142" s="8">
         <f t="shared" si="2"/>
         <v>0.95277450358187599</v>
       </c>
@@ -3694,10 +4008,10 @@
       <c r="A143" t="s">
         <v>168</v>
       </c>
-      <c r="B143" s="5">
+      <c r="B143" s="4">
         <v>2.5862947498380098E-2</v>
       </c>
-      <c r="C143" s="9">
+      <c r="C143" s="8">
         <f t="shared" si="2"/>
         <v>2.58629474983801</v>
       </c>
@@ -3706,10 +4020,10 @@
       <c r="A144" t="s">
         <v>33</v>
       </c>
-      <c r="B144" s="5">
+      <c r="B144" s="4">
         <v>4.6073174716479801E-2</v>
       </c>
-      <c r="C144" s="9">
+      <c r="C144" s="8">
         <f t="shared" si="2"/>
         <v>4.6073174716479803</v>
       </c>
@@ -3718,10 +4032,10 @@
       <c r="A145" t="s">
         <v>130</v>
       </c>
-      <c r="B145" s="5">
+      <c r="B145" s="4">
         <v>1.7331234712212401E-2</v>
       </c>
-      <c r="C145" s="9">
+      <c r="C145" s="8">
         <f t="shared" si="2"/>
         <v>1.7331234712212402</v>
       </c>
@@ -3730,10 +4044,10 @@
       <c r="A146" t="s">
         <v>131</v>
       </c>
-      <c r="B146" s="5">
+      <c r="B146" s="4">
         <v>2.9678423294092799E-3</v>
       </c>
-      <c r="C146" s="11">
+      <c r="C146" s="10">
         <f t="shared" si="2"/>
         <v>0.29678423294092798</v>
       </c>
@@ -3742,10 +4056,10 @@
       <c r="A147" t="s">
         <v>132</v>
       </c>
-      <c r="B147" s="5">
+      <c r="B147" s="4">
         <v>6.4265693736206505E-4</v>
       </c>
-      <c r="C147" s="10">
+      <c r="C147" s="9">
         <f t="shared" si="2"/>
         <v>6.4265693736206511E-2</v>
       </c>
@@ -3754,10 +4068,10 @@
       <c r="A148" t="s">
         <v>133</v>
       </c>
-      <c r="B148" s="5">
+      <c r="B148" s="4">
         <v>1.7475707470093201E-4</v>
       </c>
-      <c r="C148" s="10">
+      <c r="C148" s="9">
         <f t="shared" si="2"/>
         <v>1.7475707470093201E-2</v>
       </c>
@@ -3766,10 +4080,10 @@
       <c r="A149" t="s">
         <v>134</v>
       </c>
-      <c r="B149" s="5">
+      <c r="B149" s="4">
         <v>1.8427212641002898E-2</v>
       </c>
-      <c r="C149" s="9">
+      <c r="C149" s="8">
         <f t="shared" si="2"/>
         <v>1.8427212641002899</v>
       </c>
@@ -3778,10 +4092,10 @@
       <c r="A150" t="s">
         <v>135</v>
       </c>
-      <c r="B150" s="5">
+      <c r="B150" s="4">
         <v>3.5463224636623201E-3</v>
       </c>
-      <c r="C150" s="11">
+      <c r="C150" s="10">
         <f t="shared" si="2"/>
         <v>0.35463224636623203</v>
       </c>
@@ -3790,10 +4104,10 @@
       <c r="A151" t="s">
         <v>136</v>
       </c>
-      <c r="B151" s="5">
+      <c r="B151" s="4">
         <v>7.16328467158735E-4</v>
       </c>
-      <c r="C151" s="10">
+      <c r="C151" s="9">
         <f t="shared" si="2"/>
         <v>7.1632846715873499E-2</v>
       </c>
@@ -3802,10 +4116,10 @@
       <c r="A152" t="s">
         <v>137</v>
       </c>
-      <c r="B152" s="5">
+      <c r="B152" s="4">
         <v>1.8149606932037701E-4</v>
       </c>
-      <c r="C152" s="10">
+      <c r="C152" s="9">
         <f t="shared" si="2"/>
         <v>1.8149606932037699E-2</v>
       </c>
@@ -3814,10 +4128,10 @@
       <c r="A153" t="s">
         <v>138</v>
       </c>
-      <c r="B153" s="5">
+      <c r="B153" s="4">
         <v>1.8688418555348099E-2</v>
       </c>
-      <c r="C153" s="9">
+      <c r="C153" s="8">
         <f t="shared" si="2"/>
         <v>1.8688418555348099</v>
       </c>
@@ -3826,10 +4140,10 @@
       <c r="A154" t="s">
         <v>139</v>
       </c>
-      <c r="B154" s="5">
+      <c r="B154" s="4">
         <v>3.6141239227516801E-3</v>
       </c>
-      <c r="C154" s="11">
+      <c r="C154" s="10">
         <f t="shared" si="2"/>
         <v>0.36141239227516803</v>
       </c>
@@ -3838,10 +4152,10 @@
       <c r="A155" t="s">
         <v>140</v>
       </c>
-      <c r="B155" s="5">
+      <c r="B155" s="4">
         <v>7.0594374554003303E-4</v>
       </c>
-      <c r="C155" s="10">
+      <c r="C155" s="9">
         <f t="shared" si="2"/>
         <v>7.0594374554003303E-2</v>
       </c>
@@ -3850,10 +4164,10 @@
       <c r="A156" t="s">
         <v>141</v>
       </c>
-      <c r="B156" s="5">
+      <c r="B156" s="4">
         <v>3.8276112545634E-4</v>
       </c>
-      <c r="C156" s="10">
+      <c r="C156" s="9">
         <f t="shared" si="2"/>
         <v>3.8276112545633997E-2</v>
       </c>
@@ -3862,10 +4176,10 @@
       <c r="A157" t="s">
         <v>142</v>
       </c>
-      <c r="B157" s="5">
+      <c r="B157" s="4">
         <v>1.6151020307823699E-2</v>
       </c>
-      <c r="C157" s="9">
+      <c r="C157" s="8">
         <f t="shared" si="2"/>
         <v>1.6151020307823698</v>
       </c>
@@ -3874,10 +4188,10 @@
       <c r="A158" t="s">
         <v>143</v>
       </c>
-      <c r="B158" s="5">
+      <c r="B158" s="4">
         <v>3.4697079814773198E-3</v>
       </c>
-      <c r="C158" s="11">
+      <c r="C158" s="10">
         <f t="shared" si="2"/>
         <v>0.34697079814773196</v>
       </c>
@@ -3886,10 +4200,10 @@
       <c r="A159" t="s">
         <v>144</v>
       </c>
-      <c r="B159" s="5">
+      <c r="B159" s="4">
         <v>1.78657243568498E-3</v>
       </c>
-      <c r="C159" s="11">
+      <c r="C159" s="10">
         <f t="shared" si="2"/>
         <v>0.17865724356849799</v>
       </c>
@@ -3898,10 +4212,10 @@
       <c r="A160" t="s">
         <v>145</v>
       </c>
-      <c r="B160" s="5">
+      <c r="B160" s="4">
         <v>1.4140335261139201E-3</v>
       </c>
-      <c r="C160" s="11">
+      <c r="C160" s="10">
         <f t="shared" si="2"/>
         <v>0.141403352611392</v>
       </c>
@@ -3910,10 +4224,10 @@
       <c r="A161" t="s">
         <v>146</v>
       </c>
-      <c r="B161" s="5">
+      <c r="B161" s="4">
         <v>1.7392422586568299E-2</v>
       </c>
-      <c r="C161" s="9">
+      <c r="C161" s="8">
         <f t="shared" si="2"/>
         <v>1.7392422586568299</v>
       </c>
@@ -3922,10 +4236,10 @@
       <c r="A162" t="s">
         <v>147</v>
       </c>
-      <c r="B162" s="5">
+      <c r="B162" s="4">
         <v>4.53480011346273E-3</v>
       </c>
-      <c r="C162" s="11">
+      <c r="C162" s="10">
         <f t="shared" si="2"/>
         <v>0.45348001134627297</v>
       </c>
@@ -3934,10 +4248,10 @@
       <c r="A163" t="s">
         <v>148</v>
       </c>
-      <c r="B163" s="5">
+      <c r="B163" s="4">
         <v>2.25707967834221E-3</v>
       </c>
-      <c r="C163" s="11">
+      <c r="C163" s="10">
         <f t="shared" si="2"/>
         <v>0.22570796783422101</v>
       </c>
@@ -3946,10 +4260,10 @@
       <c r="A164" t="s">
         <v>149</v>
       </c>
-      <c r="B164" s="5">
+      <c r="B164" s="4">
         <v>1.7552509697008299E-3</v>
       </c>
-      <c r="C164" s="11">
+      <c r="C164" s="10">
         <f t="shared" si="2"/>
         <v>0.17552509697008301</v>
       </c>
@@ -3958,10 +4272,10 @@
       <c r="A165" t="s">
         <v>150</v>
       </c>
-      <c r="B165" s="5">
+      <c r="B165" s="4">
         <v>1.7379484650771802E-2</v>
       </c>
-      <c r="C165" s="9">
+      <c r="C165" s="8">
         <f t="shared" si="2"/>
         <v>1.7379484650771801</v>
       </c>
@@ -3970,10 +4284,10 @@
       <c r="A166" t="s">
         <v>151</v>
       </c>
-      <c r="B166" s="5">
+      <c r="B166" s="4">
         <v>4.3330423170439402E-3</v>
       </c>
-      <c r="C166" s="11">
+      <c r="C166" s="10">
         <f t="shared" si="2"/>
         <v>0.43330423170439403</v>
       </c>
@@ -3982,10 +4296,10 @@
       <c r="A167" t="s">
         <v>152</v>
       </c>
-      <c r="B167" s="5">
+      <c r="B167" s="4">
         <v>2.0887758218648802E-3</v>
       </c>
-      <c r="C167" s="11">
+      <c r="C167" s="10">
         <f t="shared" si="2"/>
         <v>0.20887758218648803</v>
       </c>
@@ -3994,10 +4308,10 @@
       <c r="A168" t="s">
         <v>153</v>
       </c>
-      <c r="B168" s="5">
+      <c r="B168" s="4">
         <v>1.64085506904245E-3</v>
       </c>
-      <c r="C168" s="11">
+      <c r="C168" s="10">
         <f t="shared" si="2"/>
         <v>0.164085506904245</v>
       </c>

</xml_diff>

<commit_message>
Altered files to allow for multiple light directions
</commit_message>
<xml_diff>
--- a/MATLAB/FDTD/DataPath.xlsx
+++ b/MATLAB/FDTD/DataPath.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git Hub\Ernest\MATLAB\FDTD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Ernest\MATLAB\FDTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="210">
   <si>
     <t>Simulation Folder</t>
   </si>
@@ -633,6 +633,24 @@
   </si>
   <si>
     <t>K:\FDTD\10-12-14  triangle grating in waveguide on glass slab from MATLAB suggestion #3 700-1200nm slender.xf\Simulations\000002\Run0001\output</t>
+  </si>
+  <si>
+    <t>Ex Coefficient</t>
+  </si>
+  <si>
+    <t>Ey Coefficient</t>
+  </si>
+  <si>
+    <t>Ez Coefficient</t>
+  </si>
+  <si>
+    <t>Hx Coefficient</t>
+  </si>
+  <si>
+    <t>Hy Coefficient</t>
+  </si>
+  <si>
+    <t>Hz Coefficient</t>
   </si>
 </sst>
 </file>
@@ -1125,12 +1143,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,9 +1166,15 @@
     <col min="12" max="12" width="46.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="16" max="16" width="10.21875" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" customWidth="1"/>
+    <col min="18" max="18" width="11" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1193,8 +1217,26 @@
       <c r="N1" s="17" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -1237,8 +1279,26 @@
       <c r="N2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -1281,8 +1341,26 @@
       <c r="N3" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -1325,8 +1403,26 @@
       <c r="N4" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -1369,8 +1465,26 @@
       <c r="N5" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -1413,8 +1527,26 @@
       <c r="N6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>193</v>
       </c>
@@ -1457,8 +1589,26 @@
       <c r="N7" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>196</v>
       </c>
@@ -1501,8 +1651,26 @@
       <c r="N8" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>198</v>
       </c>
@@ -1545,8 +1713,26 @@
       <c r="N9" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>200</v>
       </c>
@@ -1590,8 +1776,26 @@
       <c r="N10" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>203</v>
       </c>
@@ -1633,6 +1837,24 @@
       </c>
       <c r="N11" t="s">
         <v>187</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added RCWA and TMM, fixed FDTD
Fixed FDTD from whatever we did to it a couple weekends ago with Adam to
try to analyze single frequency FDTD, now works great.
</commit_message>
<xml_diff>
--- a/MATLAB/FDTD/DataPath.xlsx
+++ b/MATLAB/FDTD/DataPath.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Ernest\MATLAB\FDTD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Git Hub\Ernest\MATLAB\FDTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="259">
   <si>
     <t>Simulation Folder</t>
   </si>
@@ -651,6 +651,153 @@
   </si>
   <si>
     <t>Hz Coefficient</t>
+  </si>
+  <si>
+    <t>K:\Antropy\ARC waveguide 2_2 with slanted mirror one end long waveguide material below.xf\Simulations\000007\Run0001\output</t>
+  </si>
+  <si>
+    <t>S2F design +x direction</t>
+  </si>
+  <si>
+    <t>MultiPoint__X_sensor_4_transient_</t>
+  </si>
+  <si>
+    <t>Free Space 400 to 1300 5 nm mesh</t>
+  </si>
+  <si>
+    <t>K:\FDTD\Free space 400 to 1300.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>K:\FDTD\S2F_10_12_14.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>S2F design +x direction 400 to 1300 nm</t>
+  </si>
+  <si>
+    <t>N:\Kat FDTD Data\Analyzed Data\Frequency Response\Free Space 400 to 1300 5 nm mesh.mat</t>
+  </si>
+  <si>
+    <t>Info file stub</t>
+  </si>
+  <si>
+    <t>MultiPoint_Reflected_Light_Top_0_info.bin</t>
+  </si>
+  <si>
+    <t>MultiPoint__X_sensor_4_info.bin</t>
+  </si>
+  <si>
+    <t>N:\Kat FDTD Data\SunPower\Free Space 1000 to 1300 nm.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>Free Space 1000 to 1300 nm 5 nm mesh</t>
+  </si>
+  <si>
+    <t>N:\Kat FDTD Data\Analyzed Data\Frequency Response\Free Space 1000 to 1300 nm 5 nm mesh</t>
+  </si>
+  <si>
+    <t>Copper back one finger full size 10-14-14 mesh 90 nm</t>
+  </si>
+  <si>
+    <t>N:\Kat FDTD Data\SunPower\Cu metalization confidential full size one finger.xf\Simulations\000005\Run0001\output</t>
+  </si>
+  <si>
+    <t>M:\FDTD\Adam\post_array.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>Adam's post array</t>
+  </si>
+  <si>
+    <t>M:\FDTD\Adam\freespace_sinusoid_1micron.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>sinusoidal freespace at 1 micron</t>
+  </si>
+  <si>
+    <t>M:\FDTD\Adam\Analyzed data\Frequency Response</t>
+  </si>
+  <si>
+    <t>M:\FDTD\Adam\silver_tri_700_1200.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>M:\FDTD\Adam\Analyzed data\Frequency Response\sinusoidal freespace at 1 micron.mat</t>
+  </si>
+  <si>
+    <t>Mirror grating waveguide glass 1000 nm input sinusoid</t>
+  </si>
+  <si>
+    <t>M:\FDTD\Adam\silver_tri_700_1200.xf\Simulations\000002\Run0001\output</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000002\Run0001\output</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000002\Run0002\output</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000002\Run0003\output</t>
+  </si>
+  <si>
+    <t>Free Space 400-500 nm</t>
+  </si>
+  <si>
+    <t>Free Space 500-600 nm</t>
+  </si>
+  <si>
+    <t>Free Space 600-700 nm</t>
+  </si>
+  <si>
+    <t>Free Space 700-800 nm</t>
+  </si>
+  <si>
+    <t>Free Space 800-900 nm</t>
+  </si>
+  <si>
+    <t>Free Space 900-1000 nm</t>
+  </si>
+  <si>
+    <t>Free Space 1000-1100 nm</t>
+  </si>
+  <si>
+    <t>Free Space 1100-1200 nm</t>
+  </si>
+  <si>
+    <t>Free Space 1200-1300 nm</t>
+  </si>
+  <si>
+    <t>S:\Analyzed Data\Frequency Response</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000004\Run0001\output</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000004\Run0002\output</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000004\Run0006\output</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000004\Run0003\output</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000004\Run0004\output</t>
+  </si>
+  <si>
+    <t>S:\Free Space.xf\Simulations\000004\Run0005\output</t>
+  </si>
+  <si>
+    <t>K:\FDTD\Cu confidential one finger with top texture Si-SiN.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>Cu one finger with top texture SiN-Si</t>
+  </si>
+  <si>
+    <t>S:\Analyzed data\Frequency Response</t>
+  </si>
+  <si>
+    <t>S:\Cu confidential one finger with top texture SiN-Si small approximation.xf\Simulations\000001\Run0001\output</t>
+  </si>
+  <si>
+    <t>Cu one finger with top texture SiN-Si Small Approximation</t>
   </si>
 </sst>
 </file>
@@ -1143,12 +1290,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,9 +1319,10 @@
     <col min="18" max="18" width="11" customWidth="1"/>
     <col min="19" max="19" width="11.33203125" customWidth="1"/>
     <col min="20" max="20" width="10.44140625" customWidth="1"/>
+    <col min="21" max="21" width="37.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1235,8 +1383,11 @@
       <c r="T1" s="17" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U1" s="17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -1297,8 +1448,11 @@
       <c r="T2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -1359,8 +1513,11 @@
       <c r="T3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -1421,8 +1578,11 @@
       <c r="T4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -1483,8 +1643,11 @@
       <c r="T5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -1545,8 +1708,11 @@
       <c r="T6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>193</v>
       </c>
@@ -1607,8 +1773,11 @@
       <c r="T7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>196</v>
       </c>
@@ -1669,8 +1838,11 @@
       <c r="T8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>198</v>
       </c>
@@ -1731,8 +1903,11 @@
       <c r="T9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>200</v>
       </c>
@@ -1794,8 +1969,11 @@
       <c r="T10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>203</v>
       </c>
@@ -1812,7 +1990,7 @@
         <v>1.9258299999999999E-17</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>700</v>
@@ -1855,6 +2033,529 @@
       </c>
       <c r="T11">
         <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D12">
+        <v>12000</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.7314999999999999E-16</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1000</v>
+      </c>
+      <c r="H12">
+        <v>1050</v>
+      </c>
+      <c r="I12">
+        <v>166</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>180</v>
+      </c>
+      <c r="L12" t="s">
+        <v>169</v>
+      </c>
+      <c r="M12" t="s">
+        <v>212</v>
+      </c>
+      <c r="N12" t="s">
+        <v>212</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D13">
+        <v>25000</v>
+      </c>
+      <c r="E13" s="2">
+        <v>6.7392500000000003E-17</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>400</v>
+      </c>
+      <c r="H13">
+        <v>1300</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>217</v>
+      </c>
+      <c r="L13" t="s">
+        <v>169</v>
+      </c>
+      <c r="M13" t="s">
+        <v>212</v>
+      </c>
+      <c r="N13" t="s">
+        <v>212</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>100000</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.5405899999999999E-16</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="H14">
+        <v>1300</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>223</v>
+      </c>
+      <c r="L14" t="s">
+        <v>169</v>
+      </c>
+      <c r="M14" t="s">
+        <v>188</v>
+      </c>
+      <c r="N14" t="s">
+        <v>187</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15">
+        <v>1.5</v>
+      </c>
+      <c r="D15">
+        <v>7200</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.9258299999999999E-17</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>400</v>
+      </c>
+      <c r="H15">
+        <v>1300</v>
+      </c>
+      <c r="I15">
+        <v>160</v>
+      </c>
+      <c r="J15">
+        <v>160</v>
+      </c>
+      <c r="K15" t="s">
+        <v>217</v>
+      </c>
+      <c r="L15" t="s">
+        <v>169</v>
+      </c>
+      <c r="M15" t="s">
+        <v>188</v>
+      </c>
+      <c r="N15" t="s">
+        <v>187</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>50000</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4.8145800000000002E-17</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1000</v>
+      </c>
+      <c r="H16">
+        <v>1000</v>
+      </c>
+      <c r="I16">
+        <v>104</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>232</v>
+      </c>
+      <c r="L16" t="s">
+        <v>230</v>
+      </c>
+      <c r="M16" t="s">
+        <v>188</v>
+      </c>
+      <c r="N16" t="s">
+        <v>188</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>10000</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4.8145800000000002E-17</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1000</v>
+      </c>
+      <c r="H17">
+        <v>1000</v>
+      </c>
+      <c r="I17">
+        <v>104</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
+        <v>232</v>
+      </c>
+      <c r="L17" t="s">
+        <v>230</v>
+      </c>
+      <c r="M17" t="s">
+        <v>188</v>
+      </c>
+      <c r="N17" t="s">
+        <v>188</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" t="s">
+        <v>255</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>153900</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.07842E-16</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1000</v>
+      </c>
+      <c r="H18">
+        <v>1300</v>
+      </c>
+      <c r="I18">
+        <v>4000</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>223</v>
+      </c>
+      <c r="L18" t="s">
+        <v>256</v>
+      </c>
+      <c r="M18" t="s">
+        <v>188</v>
+      </c>
+      <c r="N18" t="s">
+        <v>187</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>257</v>
+      </c>
+      <c r="B19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>44600</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.0780700000000001E-16</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1000</v>
+      </c>
+      <c r="H19">
+        <v>1300</v>
+      </c>
+      <c r="I19">
+        <v>1000</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19" t="s">
+        <v>223</v>
+      </c>
+      <c r="L19" t="s">
+        <v>256</v>
+      </c>
+      <c r="M19" t="s">
+        <v>188</v>
+      </c>
+      <c r="N19" t="s">
+        <v>187</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1865,12 +2566,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1885,9 +2586,16 @@
     <col min="11" max="11" width="46.109375" customWidth="1"/>
     <col min="12" max="12" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
+    <col min="15" max="15" width="10.21875" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" customWidth="1"/>
+    <col min="19" max="19" width="10.44140625" customWidth="1"/>
+    <col min="20" max="20" width="37.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1927,8 +2635,29 @@
       <c r="M1" s="17" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -1968,8 +2697,29 @@
       <c r="M2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -2008,6 +2758,771 @@
       </c>
       <c r="M3" t="s">
         <v>191</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1700</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9.6291700000000004E-18</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>400</v>
+      </c>
+      <c r="H4">
+        <v>1300</v>
+      </c>
+      <c r="I4">
+        <v>200</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>169</v>
+      </c>
+      <c r="L4" t="s">
+        <v>188</v>
+      </c>
+      <c r="M4" t="s">
+        <v>187</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>9600</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9.6291700000000004E-18</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5">
+        <v>1300</v>
+      </c>
+      <c r="I5">
+        <v>200</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>169</v>
+      </c>
+      <c r="L5" t="s">
+        <v>188</v>
+      </c>
+      <c r="M5" t="s">
+        <v>187</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3000</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.8145800000000002E-17</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1000</v>
+      </c>
+      <c r="H6">
+        <v>1000</v>
+      </c>
+      <c r="I6">
+        <v>104</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>230</v>
+      </c>
+      <c r="L6" t="s">
+        <v>188</v>
+      </c>
+      <c r="M6" t="s">
+        <v>187</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>4700</v>
+      </c>
+      <c r="E7" s="2">
+        <v>9.6291700000000004E-18</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="H7">
+        <v>500</v>
+      </c>
+      <c r="I7">
+        <v>200</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>247</v>
+      </c>
+      <c r="L7" t="s">
+        <v>188</v>
+      </c>
+      <c r="M7" t="s">
+        <v>187</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>6800</v>
+      </c>
+      <c r="E8" s="2">
+        <v>9.6291700000000004E-18</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>500</v>
+      </c>
+      <c r="H8">
+        <v>600</v>
+      </c>
+      <c r="I8">
+        <v>200</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>247</v>
+      </c>
+      <c r="L8" t="s">
+        <v>188</v>
+      </c>
+      <c r="M8" t="s">
+        <v>187</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>9300</v>
+      </c>
+      <c r="E9" s="2">
+        <v>9.6291700000000004E-18</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>600</v>
+      </c>
+      <c r="H9">
+        <v>700</v>
+      </c>
+      <c r="I9">
+        <v>200</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>247</v>
+      </c>
+      <c r="L9" t="s">
+        <v>188</v>
+      </c>
+      <c r="M9" t="s">
+        <v>187</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>6200</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.9258299999999999E-17</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>700</v>
+      </c>
+      <c r="H10">
+        <v>800</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>247</v>
+      </c>
+      <c r="L10" t="s">
+        <v>188</v>
+      </c>
+      <c r="M10" t="s">
+        <v>187</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>7900</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.9258299999999999E-17</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>800</v>
+      </c>
+      <c r="H11">
+        <v>900</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>247</v>
+      </c>
+      <c r="L11" t="s">
+        <v>188</v>
+      </c>
+      <c r="M11" t="s">
+        <v>187</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>9900</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.9258299999999999E-17</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>900</v>
+      </c>
+      <c r="H12">
+        <v>1000</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>247</v>
+      </c>
+      <c r="L12" t="s">
+        <v>188</v>
+      </c>
+      <c r="M12" t="s">
+        <v>187</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>12000</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.9258299999999999E-17</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+      <c r="H13">
+        <v>1100</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>247</v>
+      </c>
+      <c r="L13" t="s">
+        <v>188</v>
+      </c>
+      <c r="M13" t="s">
+        <v>187</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>14300</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.9258299999999999E-17</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1100</v>
+      </c>
+      <c r="H14">
+        <v>1200</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>247</v>
+      </c>
+      <c r="L14" t="s">
+        <v>188</v>
+      </c>
+      <c r="M14" t="s">
+        <v>187</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B15" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>16900</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.9258299999999999E-17</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1200</v>
+      </c>
+      <c r="H15">
+        <v>1300</v>
+      </c>
+      <c r="I15">
+        <v>100</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>247</v>
+      </c>
+      <c r="L15" t="s">
+        <v>188</v>
+      </c>
+      <c r="M15" t="s">
+        <v>187</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>